<commit_message>
Update using data table
</commit_message>
<xml_diff>
--- a/EXCEL-CHALLENGE-28.xlsx
+++ b/EXCEL-CHALLENGE-28.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8515F6F7-3C1E-4F74-ADF7-80BCFE2B33B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{8515F6F7-3C1E-4F74-ADF7-80BCFE2B33B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F062DCF-3623-44EC-8384-1C09DE7B1196}"/>
   <bookViews>
-    <workbookView xWindow="-25695" yWindow="3465" windowWidth="23700" windowHeight="15555" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,6 +35,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t>FROM:</t>
   </si>
@@ -666,7 +668,7 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -680,7 +682,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="17"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -714,13 +715,13 @@
     <xf numFmtId="0" fontId="18" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
@@ -1492,7 +1493,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1784,10 +1785,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B1:K26"/>
+  <dimension ref="B1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1796,18 +1797,20 @@
     <col min="6" max="6" width="11.109375" customWidth="1"/>
     <col min="7" max="7" width="17.88671875" customWidth="1"/>
     <col min="8" max="8" width="25.5546875" customWidth="1"/>
+    <col min="11" max="11" width="32.5546875" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:13" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="25" t="s">
@@ -1815,107 +1818,237 @@
       </c>
       <c r="H2" s="26"/>
     </row>
-    <row r="3" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="16" t="s">
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="str" cm="1">
+        <f t="array" ref="K3">_xlfn.REDUCE(J3,$B$2:$B$16,_xlfn.LAMBDA(_xlpm.a,_xlpm.b,IF(COUNT(_xlfn.XMATCH(_xlfn.TEXTSPLIT(_xlpm.a,","),_xlfn.TEXTSPLIT(_xlpm.b,","))),_xlpm.a&amp;","&amp;_xlpm.b,_xlpm.a)))</f>
+        <v>9,18,9,17,9,18</v>
+      </c>
+      <c r="L3" t="str" cm="1">
+        <f t="array" ref="L3">_xlfn.TEXTJOIN(",",,_xlfn._xlws.SORT(_xlfn.UNIQUE(--_xlfn.TEXTSPLIT(K3,","),TRUE),,,TRUE))</f>
+        <v>9,17,18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="20">
         <v>1</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="16" t="s">
+    <row r="5" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="20">
         <v>2</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="21" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="15" t="s">
+      <c r="L5" t="str">
+        <f>L3</f>
+        <v>9,17,18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="20">
         <v>3</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="15" t="s">
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="dataTable" ref="L6:L20" dt2D="0" dtr="0" r1="J3"/>
+        <v>1,2,3,4,5,10,11,19</v>
+      </c>
+      <c r="M6" t="str" cm="1">
+        <f t="array" ref="M6:M10">_xlfn.UNIQUE(L6:L20)</f>
+        <v>1,2,3,4,5,10,11,19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="22">
         <v>4</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="23" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="K7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" t="str">
+        <v>1,2,3,4,5,10,11,19</v>
+      </c>
+      <c r="M7" t="str">
+        <v>9,15,17,18,20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15" t="s">
+      <c r="K8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" t="str">
+        <v>9,15,17,18,20</v>
+      </c>
+      <c r="M8" t="str">
+        <v>6,7,8,16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="17" t="s">
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" t="str">
+        <v>9,15,17,18,20</v>
+      </c>
+      <c r="M9" t="str">
+        <v>12,13,14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="17" t="s">
+      <c r="K10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" t="str">
+        <v>1,2,3,4,5,10,11,19</v>
+      </c>
+      <c r="M10" t="str">
+        <v>9,17,18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
+      <c r="K11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" t="str">
+        <v>1,2,3,4,5,10,11,19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="16" t="s">
+      <c r="K12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" t="str">
+        <v>1,2,3,4,5,10,11,19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="18" t="s">
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" t="str">
+        <v>1,2,3,4,5,10,11,19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="18" t="s">
+      <c r="K14" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" t="str">
+        <v>6,7,8,16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="19" t="s">
+      <c r="K15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" t="str">
+        <v>6,7,8,16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" t="str">
+        <v>6,7,8,16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" t="str">
+        <v>9,15,17,18,20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" t="str">
+        <v>12,13,14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" t="str">
+        <v>12,13,14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" t="str">
+        <v>9,17,18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" cm="1">
         <f t="array" ref="B22:B26">_xlfn.REDUCE(0,B2:B16,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.LET(_xlpm.m,_xlfn.MAP(_xlpm.a,_xlfn.LAMBDA(_xlpm.b,IF(COUNT(_xlfn.XMATCH(_xlfn.TEXTSPLIT(_xlpm.v,","),_xlfn.TEXTSPLIT(_xlpm.b,","))),_xlpm.b&amp;","&amp;_xlpm.v,_xlpm.b))),IF(AND(_xlpm.m=_xlpm.a),_xlfn.VSTACK(_xlpm.m,_xlpm.v),_xlpm.m))))</f>
         <v>0</v>
@@ -1934,7 +2067,7 @@
 o,IF(AND(m=a),VSTACK(m,v),m),MAP(o,LAMBDA(p,TEXTJOIN(",",,UNIQUE(TEXTSPLIT(p,,",")))))))),1),HSTACK(SEQUENCE(ROWS(d)),d))</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <v>1,2,4,1,3,2,3,5,2,4,3,10,11,3,19</v>
       </c>
@@ -1945,7 +2078,7 @@
         <v>17,15,20,9,18</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <v>17,15,17,20,9,17,9,18</v>
       </c>
@@ -1956,7 +2089,7 @@
         <v>6,16,7,8</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <v>6,16,6,7,8,7,16</v>
       </c>
@@ -1967,7 +2100,7 @@
         <v>12,13,14</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <v>12,13,12,14</v>
       </c>
@@ -2166,19 +2299,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -2186,11 +2315,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -2198,19 +2326,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -2218,11 +2342,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -2230,19 +2353,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -2250,11 +2369,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -2262,13 +2380,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Identified problem with direction of formation
</commit_message>
<xml_diff>
--- a/EXCEL-CHALLENGE-28.xlsx
+++ b/EXCEL-CHALLENGE-28.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{8515F6F7-3C1E-4F74-ADF7-80BCFE2B33B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F062DCF-3623-44EC-8384-1C09DE7B1196}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{8515F6F7-3C1E-4F74-ADF7-80BCFE2B33B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8D2022B-26F9-4114-887F-66D113FE20D7}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="9" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>FROM:</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>The direction of search is important.</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
@@ -364,7 +370,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,6 +462,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBFFEB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -668,7 +692,7 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -722,6 +746,11 @@
     <xf numFmtId="0" fontId="16" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
@@ -1001,11 +1030,11 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF99CCFF"/>
+      <color rgb="FFEBFFEB"/>
       <color rgb="FFFFBDFF"/>
       <color rgb="FFCCFFCC"/>
-      <color rgb="FFEBFFEB"/>
       <color rgb="FFFF9999"/>
-      <color rgb="FF99CCFF"/>
       <color rgb="FFEFFFEF"/>
     </mruColors>
   </colors>
@@ -1031,9 +1060,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>286218</xdr:colOff>
+      <xdr:colOff>282408</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>211639</xdr:rowOff>
+      <xdr:rowOff>207829</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1075,9 +1104,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>438708</xdr:colOff>
+      <xdr:colOff>434898</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>91462</xdr:rowOff>
+      <xdr:rowOff>95272</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1493,7 +1522,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1785,10 +1814,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B1:M26"/>
+  <dimension ref="B1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1797,11 +1826,14 @@
     <col min="6" max="6" width="11.109375" customWidth="1"/>
     <col min="7" max="7" width="17.88671875" customWidth="1"/>
     <col min="8" max="8" width="25.5546875" customWidth="1"/>
-    <col min="11" max="11" width="32.5546875" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="20.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.21875" customWidth="1"/>
+    <col min="14" max="14" width="19.88671875" customWidth="1"/>
+    <col min="15" max="15" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="13" t="s">
         <v>27</v>
       </c>
@@ -1809,7 +1841,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
         <v>28</v>
       </c>
@@ -1818,7 +1850,7 @@
       </c>
       <c r="H2" s="26"/>
     </row>
-    <row r="3" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
         <v>29</v>
       </c>
@@ -1831,16 +1863,19 @@
       <c r="J3" t="s">
         <v>42</v>
       </c>
-      <c r="K3" t="str" cm="1">
+      <c r="K3" s="31" t="str" cm="1">
         <f t="array" ref="K3">_xlfn.REDUCE(J3,$B$2:$B$16,_xlfn.LAMBDA(_xlpm.a,_xlpm.b,IF(COUNT(_xlfn.XMATCH(_xlfn.TEXTSPLIT(_xlpm.a,","),_xlfn.TEXTSPLIT(_xlpm.b,","))),_xlpm.a&amp;","&amp;_xlpm.b,_xlpm.a)))</f>
         <v>9,18,9,17,9,18</v>
       </c>
-      <c r="L3" t="str" cm="1">
+      <c r="L3" s="31" t="str" cm="1">
         <f t="array" ref="L3">_xlfn.TEXTJOIN(",",,_xlfn._xlws.SORT(_xlfn.UNIQUE(--_xlfn.TEXTSPLIT(K3,","),TRUE),,,TRUE))</f>
         <v>9,17,18</v>
       </c>
-    </row>
-    <row r="4" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="M3" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B4" s="15" t="s">
         <v>30</v>
       </c>
@@ -1850,8 +1885,10 @@
       <c r="H4" s="21" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+    </row>
+    <row r="5" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="15" t="s">
         <v>31</v>
       </c>
@@ -1861,12 +1898,21 @@
       <c r="H5" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L5" t="str">
+      <c r="K5" s="6"/>
+      <c r="L5" s="6" t="str">
         <f>L3</f>
         <v>9,17,18</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="M5" s="30"/>
+      <c r="N5" s="30" t="str">
+        <f>L3</f>
+        <v>9,17,18</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="14" t="s">
         <v>32</v>
       </c>
@@ -1876,19 +1922,27 @@
       <c r="H6" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L6" t="str">
-        <f t="dataTable" ref="L6:L20" dt2D="0" dtr="0" r1="J3"/>
+      <c r="L6" s="6" t="str">
+        <f t="dataTable" ref="L6:L20" dt2D="0" dtr="0" r1="J3" ca="1"/>
         <v>1,2,3,4,5,10,11,19</v>
       </c>
-      <c r="M6" t="str" cm="1">
+      <c r="M6" s="30" t="str" cm="1">
         <f t="array" ref="M6:M10">_xlfn.UNIQUE(L6:L20)</f>
         <v>1,2,3,4,5,10,11,19</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="N6" s="30" t="str">
+        <f t="dataTable" ref="N6:N10" dt2D="0" dtr="0" r1="J3"/>
+        <v>1,2,3,4,5,10,11,19</v>
+      </c>
+      <c r="O6" s="29" t="str" cm="1">
+        <f t="array" ref="O6:O9">_xlfn.UNIQUE(N6:N10)</f>
+        <v>1,2,3,4,5,10,11,19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B7" s="14" t="s">
         <v>33</v>
       </c>
@@ -1898,153 +1952,174 @@
       <c r="H7" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="L7" t="str">
+      <c r="L7" s="6" t="str">
         <v>1,2,3,4,5,10,11,19</v>
       </c>
-      <c r="M7" t="str">
+      <c r="M7" s="30" t="str">
         <v>9,15,17,18,20</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N7" s="30" t="str">
+        <v>9,15,17,18,20</v>
+      </c>
+      <c r="O7" s="29" t="str">
+        <v>9,15,17,18,20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L8" t="str">
+      <c r="L8" s="6" t="str">
         <v>9,15,17,18,20</v>
       </c>
-      <c r="M8" t="str">
+      <c r="M8" s="30" t="str">
         <v>6,7,8,16</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="30" t="str">
+        <v>6,7,8,16</v>
+      </c>
+      <c r="O8" s="29" t="str">
+        <v>6,7,8,16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L9" t="str">
+      <c r="L9" s="6" t="str">
         <v>9,15,17,18,20</v>
       </c>
-      <c r="M9" t="str">
+      <c r="M9" s="30" t="str">
         <v>12,13,14</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N9" s="30" t="str">
+        <v>12,13,14</v>
+      </c>
+      <c r="O9" s="29" t="str">
+        <v>12,13,14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L10" t="str">
+      <c r="L10" s="6" t="str">
         <v>1,2,3,4,5,10,11,19</v>
       </c>
-      <c r="M10" t="str">
+      <c r="M10" s="30" t="str">
         <v>9,17,18</v>
       </c>
-    </row>
-    <row r="11" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="30" t="str">
+        <v>9,15,17,18,20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L11" t="str">
+      <c r="L11" s="6" t="str">
         <v>1,2,3,4,5,10,11,19</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="L12" t="str">
+      <c r="L12" s="6" t="str">
         <v>1,2,3,4,5,10,11,19</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L13" t="str">
+      <c r="L13" s="6" t="str">
         <v>1,2,3,4,5,10,11,19</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L14" t="str">
+      <c r="L14" s="6" t="str">
         <v>6,7,8,16</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="L15" t="str">
+      <c r="L15" s="6" t="str">
         <v>6,7,8,16</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L16" t="str">
+      <c r="L16" s="6" t="str">
         <v>6,7,8,16</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="K17" t="s">
+      <c r="K17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L17" t="str">
+      <c r="L17" s="6" t="str">
         <v>9,15,17,18,20</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="K18" t="s">
+      <c r="K18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L18" t="str">
+      <c r="L18" s="6" t="str">
         <v>12,13,14</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="K19" t="s">
+      <c r="K19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L19" t="str">
+      <c r="L19" s="6" t="str">
         <v>12,13,14</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="K20" t="s">
+      <c r="K20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L20" t="str">
+      <c r="L20" s="6" t="str">
         <v>9,17,18</v>
       </c>
     </row>

</xml_diff>